<commit_message>
[Feat : KSW] Add Component of WeaponInfo.json
</commit_message>
<xml_diff>
--- a/Util/ExcelToJsonWizard.v1.0.6/excel_files/WeaponInfo.xlsx
+++ b/Util/ExcelToJsonWizard.v1.0.6/excel_files/WeaponInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\TheLegendoftheArcher_8team\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200E0BB7-A4A2-4DB2-AD82-331E6545B9E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E39602-8054-4121-AC91-F4ABA3F38C17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="11700" xr2:uid="{D406A3E0-B65F-4421-B497-016D24BFEA45}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
   <si>
     <t>key</t>
   </si>
@@ -363,6 +363,18 @@
   </si>
   <si>
     <t>이미지 인덱스</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Equip</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>착용여부</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -760,9 +772,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C57B8524-85F1-4110-B3A6-648333E84EF2}">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -778,10 +792,11 @@
     <col min="10" max="10" width="18.25" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="13" max="13" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -818,8 +833,11 @@
       <c r="L1" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M1" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -856,8 +874,11 @@
       <c r="L2" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -894,8 +915,11 @@
       <c r="L3" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M3" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1000</v>
       </c>
@@ -932,8 +956,11 @@
       <c r="L4" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M4" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1001</v>
       </c>
@@ -970,8 +997,11 @@
       <c r="L5" s="3">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M5" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>1002</v>
       </c>
@@ -1008,8 +1038,11 @@
       <c r="L6" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M6" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1003</v>
       </c>
@@ -1046,8 +1079,11 @@
       <c r="L7" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>1004</v>
       </c>
@@ -1084,8 +1120,11 @@
       <c r="L8" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>2000</v>
       </c>
@@ -1122,8 +1161,11 @@
       <c r="L9" s="3">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M9" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>2001</v>
       </c>
@@ -1160,8 +1202,11 @@
       <c r="L10" s="3">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M10" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>2002</v>
       </c>
@@ -1198,8 +1243,11 @@
       <c r="L11" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M11" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>2003</v>
       </c>
@@ -1236,8 +1284,11 @@
       <c r="L12" s="3">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M12" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>2004</v>
       </c>
@@ -1274,8 +1325,11 @@
       <c r="L13" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>3000</v>
       </c>
@@ -1312,8 +1366,11 @@
       <c r="L14" s="3">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M14" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>3001</v>
       </c>
@@ -1350,8 +1407,11 @@
       <c r="L15" s="3">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M15" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>3002</v>
       </c>
@@ -1388,8 +1448,11 @@
       <c r="L16" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M16" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>3003</v>
       </c>
@@ -1426,8 +1489,11 @@
       <c r="L17" s="3">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M17" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>3004</v>
       </c>
@@ -1464,8 +1530,11 @@
       <c r="L18" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M18" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>4000</v>
       </c>
@@ -1502,8 +1571,11 @@
       <c r="L19" s="3">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M19" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>4001</v>
       </c>
@@ -1540,8 +1612,11 @@
       <c r="L20" s="3">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M20" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>4002</v>
       </c>
@@ -1578,8 +1653,11 @@
       <c r="L21" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M21" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>4003</v>
       </c>
@@ -1616,8 +1694,11 @@
       <c r="L22" s="3">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M22" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>4004</v>
       </c>
@@ -1654,8 +1735,11 @@
       <c r="L23" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M23" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>5000</v>
       </c>
@@ -1692,8 +1776,11 @@
       <c r="L24" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M24" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>5001</v>
       </c>
@@ -1730,8 +1817,11 @@
       <c r="L25" s="3">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M25" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>5002</v>
       </c>
@@ -1768,8 +1858,11 @@
       <c r="L26" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M26" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>5003</v>
       </c>
@@ -1806,8 +1899,11 @@
       <c r="L27" s="3">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M27" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>5004</v>
       </c>
@@ -1844,8 +1940,11 @@
       <c r="L28" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M28" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>6000</v>
       </c>
@@ -1882,8 +1981,11 @@
       <c r="L29" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M29" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>6001</v>
       </c>
@@ -1920,8 +2022,11 @@
       <c r="L30" s="3">
         <v>45</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M30" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>6002</v>
       </c>
@@ -1958,8 +2063,11 @@
       <c r="L31" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M31" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>6003</v>
       </c>
@@ -1996,8 +2104,11 @@
       <c r="L32" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M32" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>6004</v>
       </c>
@@ -2034,8 +2145,11 @@
       <c r="L33" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M33" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>7000</v>
       </c>
@@ -2072,8 +2186,11 @@
       <c r="L34" s="3">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M34" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>7001</v>
       </c>
@@ -2110,8 +2227,11 @@
       <c r="L35" s="3">
         <v>46</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M35" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>7002</v>
       </c>
@@ -2148,8 +2268,11 @@
       <c r="L36" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M36" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>7003</v>
       </c>
@@ -2186,8 +2309,11 @@
       <c r="L37" s="3">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M37" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>7004</v>
       </c>
@@ -2224,32 +2350,35 @@
       <c r="L38" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M38" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F46" s="5"/>
     </row>
-    <row r="47" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F47" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Feat:KSW] Add Component in WeaponInfo(Bouncing)
</commit_message>
<xml_diff>
--- a/Util/ExcelToJsonWizard.v1.0.6/excel_files/WeaponInfo.xlsx
+++ b/Util/ExcelToJsonWizard.v1.0.6/excel_files/WeaponInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\TheLegendoftheArcher_8team\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C889EA9C-1114-4C95-850F-24BBD5913F45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C01236B-6CE2-4372-A833-C9C0CF94ADD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="11700" xr2:uid="{D406A3E0-B65F-4421-B497-016D24BFEA45}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="118">
   <si>
     <t>key</t>
   </si>
@@ -399,6 +399,18 @@
   </si>
   <si>
     <t>이것도 무기인가?</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bouncing</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>튕기는 횟수</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -798,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C57B8524-85F1-4110-B3A6-648333E84EF2}">
   <dimension ref="A1:W58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -817,10 +829,11 @@
     <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="1"/>
+    <col min="14" max="14" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -860,8 +873,11 @@
       <c r="M1" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -901,8 +917,11 @@
       <c r="M2" s="3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N2" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -942,8 +961,11 @@
       <c r="M3" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N3" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1001</v>
       </c>
@@ -983,8 +1005,11 @@
       <c r="M4" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1002</v>
       </c>
@@ -1024,8 +1049,11 @@
       <c r="M5" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>1003</v>
       </c>
@@ -1065,8 +1093,11 @@
       <c r="M6" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1004</v>
       </c>
@@ -1106,8 +1137,11 @@
       <c r="M7" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>1005</v>
       </c>
@@ -1147,8 +1181,11 @@
       <c r="M8" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>2001</v>
       </c>
@@ -1188,8 +1225,11 @@
       <c r="M9" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>2002</v>
       </c>
@@ -1229,8 +1269,11 @@
       <c r="M10" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>2003</v>
       </c>
@@ -1270,8 +1313,11 @@
       <c r="M11" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>2004</v>
       </c>
@@ -1311,8 +1357,11 @@
       <c r="M12" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>2005</v>
       </c>
@@ -1352,8 +1401,11 @@
       <c r="M13" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>3001</v>
       </c>
@@ -1393,8 +1445,11 @@
       <c r="M14" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>3002</v>
       </c>
@@ -1434,8 +1489,11 @@
       <c r="M15" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>3003</v>
       </c>
@@ -1475,8 +1533,11 @@
       <c r="M16" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N16" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>3004</v>
       </c>
@@ -1516,8 +1577,11 @@
       <c r="M17" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N17" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>3005</v>
       </c>
@@ -1557,8 +1621,11 @@
       <c r="M18" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>4001</v>
       </c>
@@ -1598,8 +1665,11 @@
       <c r="M19" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>4002</v>
       </c>
@@ -1639,8 +1709,11 @@
       <c r="M20" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>4003</v>
       </c>
@@ -1680,8 +1753,11 @@
       <c r="M21" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N21" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>4004</v>
       </c>
@@ -1721,8 +1797,11 @@
       <c r="M22" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N22" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>4005</v>
       </c>
@@ -1762,8 +1841,11 @@
       <c r="M23" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N23" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>5001</v>
       </c>
@@ -1803,8 +1885,11 @@
       <c r="M24" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>5002</v>
       </c>
@@ -1844,8 +1929,11 @@
       <c r="M25" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>5003</v>
       </c>
@@ -1885,8 +1973,11 @@
       <c r="M26" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N26" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>5004</v>
       </c>
@@ -1926,8 +2017,11 @@
       <c r="M27" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N27" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>5005</v>
       </c>
@@ -1967,8 +2061,11 @@
       <c r="M28" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N28" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>6001</v>
       </c>
@@ -2008,8 +2105,11 @@
       <c r="M29" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>6002</v>
       </c>
@@ -2049,8 +2149,11 @@
       <c r="M30" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>6003</v>
       </c>
@@ -2090,8 +2193,11 @@
       <c r="M31" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>6004</v>
       </c>
@@ -2130,6 +2236,9 @@
       </c>
       <c r="M32" s="3" t="b">
         <v>0</v>
+      </c>
+      <c r="N32" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2172,6 +2281,9 @@
       <c r="M33" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="N33" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="34" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
@@ -2213,6 +2325,9 @@
       <c r="M34" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="N34" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
@@ -2254,6 +2369,9 @@
       <c r="M35" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="N35" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
@@ -2295,6 +2413,9 @@
       <c r="M36" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="N36" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="37" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
@@ -2336,6 +2457,9 @@
       <c r="M37" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="N37" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
@@ -2377,6 +2501,9 @@
       <c r="M38" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="N38" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="39" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
@@ -2418,6 +2545,9 @@
       <c r="M39" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="N39" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40">
@@ -2459,6 +2589,9 @@
       <c r="M40" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="N40" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41">
@@ -2498,6 +2631,9 @@
         <v>96</v>
       </c>
       <c r="M41" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N41" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Feat:KSW] Add Map Prefabs, 10Stage Special Map
</commit_message>
<xml_diff>
--- a/Util/ExcelToJsonWizard.v1.0.6/excel_files/WeaponInfo.xlsx
+++ b/Util/ExcelToJsonWizard.v1.0.6/excel_files/WeaponInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\TheLegendoftheArcher_8team\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C01236B-6CE2-4372-A833-C9C0CF94ADD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186435D3-4F71-4CE0-A79E-ED1A492B1A0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="11700" xr2:uid="{D406A3E0-B65F-4421-B497-016D24BFEA45}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="119">
   <si>
     <t>key</t>
   </si>
@@ -411,6 +411,10 @@
   </si>
   <si>
     <t>튕기는 횟수</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GrenadierWeapon</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -811,7 +815,7 @@
   <dimension ref="A1:W58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2638,7 +2642,48 @@
       </c>
     </row>
     <row r="42" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F42" s="5"/>
+      <c r="A42">
+        <v>9004</v>
+      </c>
+      <c r="B42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="3">
+        <v>15</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42">
+        <v>0.5</v>
+      </c>
+      <c r="G42">
+        <v>5</v>
+      </c>
+      <c r="H42">
+        <v>7</v>
+      </c>
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="K42" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L42" s="3">
+        <v>97</v>
+      </c>
+      <c r="M42" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N42" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F43" s="5"/>

</xml_diff>